<commit_message>
Creación de transacción de pagos de creditos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\tarjetacredito\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB132A0-CDBD-4FBB-8235-10104D735156}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBFB47D-66D8-48C0-B3C5-C65ECBF1896B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -100,94 +100,89 @@
     <t>numeroCuenta</t>
   </si>
   <si>
-    <t>numeroTarjeta</t>
-  </si>
-  <si>
     <t>tipoPago</t>
   </si>
   <si>
     <t>valorPago</t>
   </si>
   <si>
-    <t>moneda</t>
-  </si>
-  <si>
     <t>22493944</t>
   </si>
   <si>
-    <t>tipoTarjeta</t>
-  </si>
-  <si>
-    <t>Personal American Express</t>
-  </si>
-  <si>
-    <t>*2736</t>
-  </si>
-  <si>
-    <t>Pago mínimo en dólares</t>
-  </si>
-  <si>
-    <t>Dolares</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
     <t>Ahorros</t>
   </si>
   <si>
     <t>Otro valor</t>
   </si>
   <si>
-    <t>*7826</t>
-  </si>
-  <si>
-    <t>Pesos</t>
-  </si>
-  <si>
-    <t>500000</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Personal Visa</t>
-  </si>
-  <si>
-    <t>*5880</t>
-  </si>
-  <si>
-    <t>480369</t>
-  </si>
-  <si>
     <t>Corriente</t>
   </si>
   <si>
-    <t>406-125170-00</t>
-  </si>
-  <si>
-    <t>406-725170-06</t>
-  </si>
-  <si>
-    <t>autotest10</t>
-  </si>
-  <si>
     <t>1234</t>
+  </si>
+  <si>
+    <t>tipoPrestamo</t>
+  </si>
+  <si>
+    <t>Crediagil</t>
+  </si>
+  <si>
+    <t>29281005217</t>
+  </si>
+  <si>
+    <t>Pago mínimo</t>
+  </si>
+  <si>
+    <t>Pago total</t>
+  </si>
+  <si>
+    <t>50893</t>
+  </si>
+  <si>
+    <t>40893</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>pruebasusuario11</t>
+  </si>
+  <si>
+    <t>numeroPrestamo</t>
+  </si>
+  <si>
+    <t>406-106940-01</t>
+  </si>
+  <si>
+    <t>406-706940-12</t>
+  </si>
+  <si>
+    <t>406-706940-13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -281,23 +276,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -603,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -624,7 +619,7 @@
     <col min="17" max="17" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -668,42 +663,39 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="10" customFormat="1">
+    <row r="2" spans="1:20" s="10" customFormat="1">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>50</v>
+      <c r="D2" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>15</v>
@@ -733,42 +725,39 @@
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>48</v>
+      <c r="T2" s="13" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:20">
       <c r="A3" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>50</v>
+      <c r="D3" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>15</v>
@@ -798,42 +787,39 @@
         <v>22</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="B4" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>50</v>
+      <c r="D4" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
@@ -863,29 +849,26 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="U4" s="12" t="s">
-        <v>49</v>
+        <v>29</v>
+      </c>
+      <c r="T4" s="13" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="N3" r:id="rId2" xr:uid="{67C6CB3E-A984-46BB-B622-F0ADD216DE02}"/>

</xml_diff>

<commit_message>
Creación de question y estabilización de pagos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBFB47D-66D8-48C0-B3C5-C65ECBF1896B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1C0175-6E15-4D79-A75B-0AF112B10912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -145,9 +145,6 @@
     <t>50893</t>
   </si>
   <si>
-    <t>40893</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -163,19 +160,35 @@
     <t>406-706940-12</t>
   </si>
   <si>
-    <t>406-706940-13</t>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>29281005233</t>
+  </si>
+  <si>
+    <t>406-107870-00</t>
+  </si>
+  <si>
+    <t>CREDIAGIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -276,22 +289,23 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -600,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -666,7 +680,7 @@
         <v>35</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>26</v>
@@ -692,7 +706,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>34</v>
@@ -734,13 +748,13 @@
         <v>38</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>33</v>
       </c>
       <c r="T2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -754,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>34</v>
@@ -802,7 +816,7 @@
         <v>29</v>
       </c>
       <c r="T3" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:20">
@@ -816,7 +830,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>34</v>
@@ -849,26 +863,26 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="13" t="s">
-        <v>47</v>
+        <v>33</v>
+      </c>
+      <c r="T4" s="14" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="N3" r:id="rId2" xr:uid="{67C6CB3E-A984-46BB-B622-F0ADD216DE02}"/>

</xml_diff>

<commit_message>
Estabilización pago de créditos
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -1,26 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/pagos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E1C0175-6E15-4D79-A75B-0AF112B10912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -163,32 +167,31 @@
     <t>1000</t>
   </si>
   <si>
-    <t>29281005233</t>
-  </si>
-  <si>
-    <t>406-107870-00</t>
-  </si>
-  <si>
-    <t>CREDIAGIL</t>
+    <t>pruebauser01</t>
+  </si>
+  <si>
+    <t>6789</t>
+  </si>
+  <si>
+    <t>Prestamo personal</t>
+  </si>
+  <si>
+    <t>29281023961</t>
+  </si>
+  <si>
+    <t>406-182800-03</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -289,27 +292,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,29 +616,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="15" width="27.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="8" width="15.5" customWidth="1"/>
+    <col min="9" max="10" width="23.5" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="15" width="27.83203125" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="25.5" customWidth="1"/>
+    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -695,7 +701,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="10" customFormat="1">
+    <row r="2" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -757,7 +763,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -819,7 +825,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -829,11 +835,11 @@
       <c r="C4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="12" t="s">
-        <v>42</v>
+      <c r="D4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
@@ -866,7 +872,7 @@
         <v>49</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>30</v>
@@ -878,15 +884,15 @@
         <v>33</v>
       </c>
       <c r="T4" s="14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="N3" r:id="rId2" xr:uid="{67C6CB3E-A984-46BB-B622-F0ADD216DE02}"/>
-    <hyperlink ref="N4" r:id="rId3" xr:uid="{BBE34ADD-6B07-4872-AD38-7133AF9FBFD6}"/>
+    <hyperlink ref="N2" r:id="rId1"/>
+    <hyperlink ref="N3" r:id="rId2"/>
+    <hyperlink ref="N4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>

</xml_diff>

<commit_message>
Estabilización de pago de tarjetas no propias
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>ID</t>
   </si>
@@ -113,9 +113,6 @@
     <t>22493944</t>
   </si>
   <si>
-    <t>Ahorros</t>
-  </si>
-  <si>
     <t>Otro valor</t>
   </si>
   <si>
@@ -128,18 +125,9 @@
     <t>Corriente</t>
   </si>
   <si>
-    <t>1234</t>
-  </si>
-  <si>
     <t>tipoPrestamo</t>
   </si>
   <si>
-    <t>Crediagil</t>
-  </si>
-  <si>
-    <t>29281005217</t>
-  </si>
-  <si>
     <t>Pago mínimo</t>
   </si>
   <si>
@@ -152,16 +140,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>pruebasusuario11</t>
-  </si>
-  <si>
     <t>numeroPrestamo</t>
-  </si>
-  <si>
-    <t>406-106940-01</t>
-  </si>
-  <si>
-    <t>406-706940-12</t>
   </si>
   <si>
     <t>1000</t>
@@ -186,26 +165,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -292,23 +257,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -619,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -683,10 +646,10 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>26</v>
@@ -711,11 +674,11 @@
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>42</v>
+      <c r="D2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>15</v>
@@ -745,27 +708,27 @@
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="S2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="12" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>28</v>
@@ -773,11 +736,11 @@
       <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>42</v>
+      <c r="D3" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>15</v>
@@ -807,27 +770,27 @@
         <v>22</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="S3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>28</v>
@@ -836,10 +799,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
@@ -869,26 +832,26 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="14" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
     <hyperlink ref="N3" r:id="rId2"/>

</xml_diff>

<commit_message>
Estabilización pago tc propias
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t>50893</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>numeroPrestamo</t>
   </si>
   <si>
@@ -159,6 +156,24 @@
   </si>
   <si>
     <t>406-182800-03</t>
+  </si>
+  <si>
+    <t>inversion2</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Prestamo personal ta</t>
+  </si>
+  <si>
+    <t>29281005510</t>
+  </si>
+  <si>
+    <t>20561111</t>
+  </si>
+  <si>
+    <t>406-130790-01</t>
   </si>
 </sst>
 </file>
@@ -583,7 +598,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -649,7 +664,7 @@
         <v>33</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>26</v>
@@ -675,10 +690,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>15</v>
@@ -708,22 +723,22 @@
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="7" t="s">
-        <v>34</v>
+        <v>47</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -737,10 +752,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>15</v>
@@ -770,13 +785,13 @@
         <v>22</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>35</v>
+      <c r="Q3" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>36</v>
@@ -785,7 +800,7 @@
         <v>32</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -799,10 +814,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>15</v>
@@ -832,22 +847,22 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>29</v>
       </c>
       <c r="R4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S4" s="10" t="s">
         <v>32</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adición de escenarios de pagos y transferencias desde cuenta sin saldo
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mruiz/Documents/ProyectosTODO1/bancolombia-app-personas-osp-tests-bdd-screen-play/APP_PERSONAS/src/test/resources/datadriven/pagos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886DC8F-06B9-4B1F-904D-015B825F8E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -174,13 +175,16 @@
   </si>
   <si>
     <t>406-130790-01</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,7 +296,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,30 +598,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
-    <col min="7" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="10" width="23.5" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="13" width="16.83203125" customWidth="1"/>
-    <col min="14" max="15" width="27.83203125" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
-    <col min="17" max="17" width="25.5" customWidth="1"/>
-    <col min="20" max="20" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
+    <col min="7" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="15" width="27.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="17" width="25.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,7 +683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" s="10" customFormat="1" ht="30">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -741,7 +745,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="30">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
@@ -803,7 +807,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="30">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
@@ -862,17 +866,80 @@
         <v>32</v>
       </c>
       <c r="T4" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="30">
+      <c r="A5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="12" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="N3" r:id="rId2"/>
-    <hyperlink ref="N4" r:id="rId3"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="N3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="N4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="N5" r:id="rId4" xr:uid="{3AD5B118-CD54-495E-8BD8-AA1C7F316868}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor general de clases, por ejecución de automatización
</commit_message>
<xml_diff>
--- a/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
+++ b/APP_PERSONAS/src/test/resources/datadriven/pagos/Creditos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\Daniel Torres Devco\todo1\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\appOSP\bancolombia-app-personas-osp-tests-bdd-screen-play\APP_PERSONAS\src\test\resources\datadriven\pagos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7886DC8F-06B9-4B1F-904D-015B825F8E64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D6CC58-4975-40AF-85CE-89D15AAE9AE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -150,9 +150,6 @@
     <t>6789</t>
   </si>
   <si>
-    <t>Prestamo personal</t>
-  </si>
-  <si>
     <t>29281023961</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>Prestamo Personal Ta</t>
+  </si>
+  <si>
+    <t>406-782800-09</t>
+  </si>
+  <si>
+    <t>Ahorros</t>
   </si>
 </sst>
 </file>
@@ -601,27 +607,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="7" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="10" width="23.42578125" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" customWidth="1"/>
-    <col min="12" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="15" width="27.85546875" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="25.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" customWidth="1"/>
+    <col min="7" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="10" width="23.453125" customWidth="1"/>
+    <col min="11" max="11" width="20.7265625" customWidth="1"/>
+    <col min="12" max="13" width="16.81640625" customWidth="1"/>
+    <col min="14" max="15" width="27.81640625" customWidth="1"/>
+    <col min="16" max="16" width="15.7265625" customWidth="1"/>
+    <col min="17" max="17" width="25.453125" customWidth="1"/>
+    <col min="20" max="20" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="10" customFormat="1" ht="30">
+    <row r="2" spans="1:20" s="10" customFormat="1" ht="29">
       <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
@@ -694,10 +700,10 @@
         <v>14</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>15</v>
@@ -727,25 +733,25 @@
         <v>22</v>
       </c>
       <c r="O2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S2" s="10" t="s">
         <v>32</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="30">
+    <row r="3" spans="1:20" ht="29">
       <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
@@ -789,10 +795,10 @@
         <v>22</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="Q3" s="7" t="s">
         <v>34</v>
@@ -804,10 +810,10 @@
         <v>32</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30">
+    <row r="4" spans="1:20" ht="29">
       <c r="A4" s="8" t="s">
         <v>31</v>
       </c>
@@ -851,10 +857,10 @@
         <v>22</v>
       </c>
       <c r="O4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="Q4" s="6" t="s">
         <v>29</v>
@@ -866,12 +872,12 @@
         <v>32</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="30">
+    <row r="5" spans="1:20" ht="29">
       <c r="A5" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>28</v>
@@ -913,10 +919,10 @@
         <v>22</v>
       </c>
       <c r="O5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>29</v>
@@ -925,10 +931,10 @@
         <v>38</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>